<commit_message>
SOCs for blood and urine samples
</commit_message>
<xml_diff>
--- a/metadata/SSD-NHANES-2017-2018-100.xlsx
+++ b/metadata/SSD-NHANES-2017-2018-100.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrique/git/nhanes-hadatac/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C96DB7C-ADC0-6146-8D7B-E9FA640AD434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38BB401B-EFDA-C843-A5A5-D3A95C0DBD75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25820" yWindow="-19720" windowWidth="27640" windowHeight="16440" xr2:uid="{99F202CB-6519-5442-830D-344A4E1B0030}"/>
+    <workbookView xWindow="-3500" yWindow="-21940" windowWidth="27640" windowHeight="16440" xr2:uid="{99F202CB-6519-5442-830D-344A4E1B0030}"/>
   </bookViews>
   <sheets>
     <sheet name="SSD" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="53">
   <si>
     <t>sheet</t>
   </si>
@@ -176,6 +176,24 @@
   </si>
   <si>
     <t>nhanes-kb:SOC-NHANES-2017-2018-HH_REF_PERSON</t>
+  </si>
+  <si>
+    <t>nhanes-kb:SOC-NHANES-2017-2018-BLOOD</t>
+  </si>
+  <si>
+    <t>??blood</t>
+  </si>
+  <si>
+    <t>Blood Sample</t>
+  </si>
+  <si>
+    <t>nhanes-kb:SOC-NHANES-2017-2018-URINE</t>
+  </si>
+  <si>
+    <t>??urine</t>
+  </si>
+  <si>
+    <t>Urine Sample</t>
   </si>
 </sst>
 </file>
@@ -527,16 +545,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B088F3-3515-904B-9B51-EE2323ADDBE3}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G6" sqref="F4:G6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
@@ -735,6 +753,40 @@
         <v>45</v>
       </c>
     </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -745,7 +797,7 @@
   <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A2" sqref="A2:A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>